<commit_message>
fixed inverse multiplied and added CNY onshore fwd pt
</commit_message>
<xml_diff>
--- a/meta/lookup_tickers.xlsx
+++ b/meta/lookup_tickers.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="132">
   <si>
     <t>Currency</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">USDCNH 12 Month Forward Points </t>
-  </si>
-  <si>
-    <t>FirstDate</t>
   </si>
   <si>
     <t>CCN12M BGN Curncy</t>
@@ -433,6 +430,12 @@
   </si>
   <si>
     <t>TMA 1Y CNH Hong Kong InterBank Offered Rate (CNH Hibor) Fixing</t>
+  </si>
+  <si>
+    <t>CCO12M BGN Curncy</t>
+  </si>
+  <si>
+    <t>CNY Onsh Comm Fwd Pt 12M</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +774,7 @@
     <col min="5" max="5" width="57.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -787,13 +790,10 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -802,15 +802,15 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -819,15 +819,15 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -836,15 +836,15 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -853,15 +853,15 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -870,27 +870,27 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -907,7 +907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -918,32 +918,32 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -952,13 +952,13 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -969,94 +969,94 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>76</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
       <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1065,15 +1065,15 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -1082,15 +1082,15 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -1099,44 +1099,44 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1158,7 +1158,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -1167,15 +1167,15 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1184,15 +1184,15 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -1201,15 +1201,15 @@
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1218,15 +1218,15 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1235,15 +1235,15 @@
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -1252,10 +1252,10 @@
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1277,24 +1277,24 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1303,32 +1303,32 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1337,15 +1337,15 @@
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s">
-        <v>126</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1354,15 +1354,15 @@
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E35" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
@@ -1371,15 +1371,15 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -1388,15 +1388,15 @@
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -1405,83 +1405,83 @@
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="E38" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="E42" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -1490,57 +1490,74 @@
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E44" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>121</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>9</v>
       </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>8</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>13</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E47" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chged AUD, KRW, NOK to source='ICPL'
</commit_message>
<xml_diff>
--- a/meta/lookup_tickers.xlsx
+++ b/meta/lookup_tickers.xlsx
@@ -273,9 +273,6 @@
     <t>COP</t>
   </si>
   <si>
-    <t>ADBS1 BGN Curncy</t>
-  </si>
-  <si>
     <t>CDBS1 BGN Curncy</t>
   </si>
   <si>
@@ -300,21 +297,12 @@
     <t>JYBS1 BGN Curncy</t>
   </si>
   <si>
-    <t>KRBS1 BGN Curncy</t>
-  </si>
-  <si>
     <t>MPBS1A BGN Curncy</t>
   </si>
   <si>
     <t>MRBS1 BGN Curncy</t>
   </si>
   <si>
-    <t>NKBS1 BGN Curncy</t>
-  </si>
-  <si>
-    <t>NDBS1 BGN Curncy</t>
-  </si>
-  <si>
     <t>RRBS1 BGN Curncy</t>
   </si>
   <si>
@@ -436,6 +424,18 @@
   </si>
   <si>
     <t>CNY Onsh Comm Fwd Pt 12M</t>
+  </si>
+  <si>
+    <t>ADBS1 ICPL Curncy</t>
+  </si>
+  <si>
+    <t>NKBS1 ICPL Curncy</t>
+  </si>
+  <si>
+    <t>NDBS1 ICPL Curncy</t>
+  </si>
+  <si>
+    <t>KRBS1 TPRA Curncy</t>
   </si>
 </sst>
 </file>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,10 +802,10 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -870,10 +870,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -935,10 +935,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -952,10 +952,10 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -969,10 +969,10 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1003,10 +1003,10 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1065,10 +1065,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1082,10 +1082,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1099,10 +1099,10 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1136,7 +1136,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1150,10 +1150,10 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1167,10 +1167,10 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1184,10 +1184,10 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1201,10 +1201,10 @@
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1218,10 +1218,10 @@
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>131</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1235,10 +1235,10 @@
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1252,10 +1252,10 @@
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1269,10 +1269,10 @@
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="E30" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1286,10 +1286,10 @@
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1354,10 +1354,10 @@
         <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1371,10 +1371,10 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1388,10 +1388,10 @@
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E37" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1405,10 +1405,10 @@
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1422,10 +1422,10 @@
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1439,10 +1439,10 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1456,10 +1456,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1490,10 +1490,10 @@
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1538,10 +1538,10 @@
         <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>